<commit_message>
Bijna klaar! Duidelijke message komt later
</commit_message>
<xml_diff>
--- a/df_features.xlsx
+++ b/df_features.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B88"/>
+  <dimension ref="A1:B76"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -448,7 +448,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>CKD-EPI eGFR</t>
+          <t>Kreatinine</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -458,7 +458,7 @@
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Gamma-GT</t>
+          <t>Length</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -468,7 +468,7 @@
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>LDH</t>
+          <t>Vrij T4</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -478,7 +478,7 @@
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>GYN</t>
+          <t>25-OH Vitamine D</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -488,7 +488,7 @@
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>Leukocyten</t>
+          <t>Neurological</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -498,7 +498,7 @@
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>25-OH Vitamine D</t>
+          <t>Trombocyten</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -508,7 +508,7 @@
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>Opnames_spec</t>
+          <t>Kalium</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -518,7 +518,7 @@
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>Kreatinine</t>
+          <t>Specialisms_hospitalization</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -528,7 +528,7 @@
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>Beeldvormende_verr</t>
+          <t>LDH</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -538,7 +538,7 @@
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>Calcium</t>
+          <t>CKD-EPI eGFR</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -548,7 +548,7 @@
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>Length</t>
+          <t>KIC</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -558,7 +558,7 @@
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>RRdiast</t>
+          <t>Glucose/PL</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -568,7 +568,7 @@
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>ASAT</t>
+          <t>Psychofarmaca</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -578,7 +578,7 @@
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
         <is>
-          <t>Anti-hypertensives</t>
+          <t>Alk.Fosf.</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -588,7 +588,7 @@
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
         <is>
-          <t>Endocrine/metabolic</t>
+          <t>Icterische index</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -598,7 +598,7 @@
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
         <is>
-          <t>Brief_GYN</t>
+          <t>Lipemische index</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -608,7 +608,7 @@
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
         <is>
-          <t>Ureum</t>
+          <t>RRdiast</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -618,7 +618,7 @@
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
         <is>
-          <t>Brief_INT</t>
+          <t>Neoplasms</t>
         </is>
       </c>
       <c r="B19" t="n">
@@ -628,7 +628,7 @@
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
         <is>
-          <t>Albumine</t>
+          <t>LON</t>
         </is>
       </c>
       <c r="B20" t="n">
@@ -638,7 +638,7 @@
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
         <is>
-          <t>TSH</t>
+          <t>Natrium</t>
         </is>
       </c>
       <c r="B21" t="n">
@@ -648,7 +648,7 @@
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
         <is>
-          <t>MCV</t>
+          <t>ALAT</t>
         </is>
       </c>
       <c r="B22" t="n">
@@ -658,47 +658,47 @@
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
         <is>
-          <t>Trombocyten</t>
+          <t>BMI</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="inlineStr">
         <is>
-          <t>KAA</t>
+          <t>LDL-Cholesterol</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="inlineStr">
         <is>
-          <t>ALAT</t>
+          <t>Radiologic_investigations</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="inlineStr">
         <is>
-          <t>Musculoskeletal</t>
+          <t>Calcium</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="inlineStr">
         <is>
-          <t>BMI</t>
+          <t>Musculoskeletal</t>
         </is>
       </c>
       <c r="B27" t="n">
@@ -708,7 +708,7 @@
     <row r="28">
       <c r="A28" s="1" t="inlineStr">
         <is>
-          <t>Genitourinary</t>
+          <t>GYN</t>
         </is>
       </c>
       <c r="B28" t="n">
@@ -718,7 +718,7 @@
     <row r="29">
       <c r="A29" s="1" t="inlineStr">
         <is>
-          <t>Brief_DER</t>
+          <t>FSH</t>
         </is>
       </c>
       <c r="B29" t="n">
@@ -728,7 +728,7 @@
     <row r="30">
       <c r="A30" s="1" t="inlineStr">
         <is>
-          <t>Congenital anomalies</t>
+          <t>ASAT</t>
         </is>
       </c>
       <c r="B30" t="n">
@@ -738,7 +738,7 @@
     <row r="31">
       <c r="A31" s="1" t="inlineStr">
         <is>
-          <t>Kalium</t>
+          <t>Leukocyten</t>
         </is>
       </c>
       <c r="B31" t="n">
@@ -748,7 +748,7 @@
     <row r="32">
       <c r="A32" s="1" t="inlineStr">
         <is>
-          <t>Specialisms_hospitalization</t>
+          <t>URO</t>
         </is>
       </c>
       <c r="B32" t="n">
@@ -758,7 +758,7 @@
     <row r="33">
       <c r="A33" s="1" t="inlineStr">
         <is>
-          <t>Neoplasms</t>
+          <t>Endocrine/metabolic</t>
         </is>
       </c>
       <c r="B33" t="n">
@@ -768,7 +768,7 @@
     <row r="34">
       <c r="A34" s="1" t="inlineStr">
         <is>
-          <t>Brief_PLA</t>
+          <t>NEU</t>
         </is>
       </c>
       <c r="B34" t="n">
@@ -778,7 +778,7 @@
     <row r="35">
       <c r="A35" s="1" t="inlineStr">
         <is>
-          <t>KNO</t>
+          <t>MCV</t>
         </is>
       </c>
       <c r="B35" t="n">
@@ -788,7 +788,7 @@
     <row r="36">
       <c r="A36" s="1" t="inlineStr">
         <is>
-          <t>Brief_MDL</t>
+          <t>RDW</t>
         </is>
       </c>
       <c r="B36" t="n">
@@ -798,67 +798,67 @@
     <row r="37">
       <c r="A37" s="1" t="inlineStr">
         <is>
-          <t>Brief_END</t>
+          <t>END</t>
         </is>
       </c>
       <c r="B37" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="inlineStr">
         <is>
-          <t>LDL-Cholesterol</t>
+          <t>KIN</t>
         </is>
       </c>
       <c r="B38" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="inlineStr">
         <is>
-          <t>Brief_NEU</t>
+          <t>Genitourinary</t>
         </is>
       </c>
       <c r="B39" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="inlineStr">
         <is>
-          <t>Radiologic_investigations</t>
+          <t>MET</t>
         </is>
       </c>
       <c r="B40" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="inlineStr">
         <is>
-          <t>Psychofarmaca</t>
+          <t>MDL</t>
         </is>
       </c>
       <c r="B41" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="inlineStr">
         <is>
-          <t>Brief_GGZ</t>
+          <t>LOG</t>
         </is>
       </c>
       <c r="B42" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="inlineStr">
         <is>
-          <t>URO</t>
+          <t>Hemolytische index</t>
         </is>
       </c>
       <c r="B43" t="n">
@@ -868,7 +868,7 @@
     <row r="44">
       <c r="A44" s="1" t="inlineStr">
         <is>
-          <t>KLG</t>
+          <t>Tot. Bilirubine</t>
         </is>
       </c>
       <c r="B44" t="n">
@@ -878,7 +878,7 @@
     <row r="45">
       <c r="A45" s="1" t="inlineStr">
         <is>
-          <t>Icterische index</t>
+          <t>SUM</t>
         </is>
       </c>
       <c r="B45" t="n">
@@ -888,7 +888,7 @@
     <row r="46">
       <c r="A46" s="1" t="inlineStr">
         <is>
-          <t>Glucose/PL</t>
+          <t>Pregnancy complications</t>
         </is>
       </c>
       <c r="B46" t="n">
@@ -898,7 +898,7 @@
     <row r="47">
       <c r="A47" s="1" t="inlineStr">
         <is>
-          <t>SUM</t>
+          <t>Total_amount_ICD10s</t>
         </is>
       </c>
       <c r="B47" t="n">
@@ -908,7 +908,7 @@
     <row r="48">
       <c r="A48" s="1" t="inlineStr">
         <is>
-          <t>RRsyst</t>
+          <t>KLG</t>
         </is>
       </c>
       <c r="B48" t="n">
@@ -918,27 +918,27 @@
     <row r="49">
       <c r="A49" s="1" t="inlineStr">
         <is>
-          <t>FSH</t>
+          <t>KCH</t>
         </is>
       </c>
       <c r="B49" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="inlineStr">
         <is>
-          <t>Natrium</t>
+          <t>Gamma-GT</t>
         </is>
       </c>
       <c r="B50" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="inlineStr">
         <is>
-          <t>Hemolytische index</t>
+          <t>RRsyst</t>
         </is>
       </c>
       <c r="B51" t="n">
@@ -948,7 +948,7 @@
     <row r="52">
       <c r="A52" s="1" t="inlineStr">
         <is>
-          <t>OCH</t>
+          <t>Hemoglobine</t>
         </is>
       </c>
       <c r="B52" t="n">
@@ -958,7 +958,7 @@
     <row r="53">
       <c r="A53" s="1" t="inlineStr">
         <is>
-          <t>END</t>
+          <t>KEN</t>
         </is>
       </c>
       <c r="B53" t="n">
@@ -968,7 +968,7 @@
     <row r="54">
       <c r="A54" s="1" t="inlineStr">
         <is>
-          <t>Tot. Bilirubine</t>
+          <t>Ureum</t>
         </is>
       </c>
       <c r="B54" t="n">
@@ -978,7 +978,7 @@
     <row r="55">
       <c r="A55" s="1" t="inlineStr">
         <is>
-          <t>Total_amount_ICD10s</t>
+          <t>ANE</t>
         </is>
       </c>
       <c r="B55" t="n">
@@ -988,7 +988,7 @@
     <row r="56">
       <c r="A56" s="1" t="inlineStr">
         <is>
-          <t>RDW</t>
+          <t>KNO</t>
         </is>
       </c>
       <c r="B56" t="n">
@@ -998,7 +998,7 @@
     <row r="57">
       <c r="A57" s="1" t="inlineStr">
         <is>
-          <t>Hemoglobine</t>
+          <t>KLZ</t>
         </is>
       </c>
       <c r="B57" t="n">
@@ -1008,17 +1008,17 @@
     <row r="58">
       <c r="A58" s="1" t="inlineStr">
         <is>
-          <t>Respiratory</t>
+          <t>NEF</t>
         </is>
       </c>
       <c r="B58" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="inlineStr">
         <is>
-          <t>RAD</t>
+          <t>ORT</t>
         </is>
       </c>
       <c r="B59" t="n">
@@ -1028,7 +1028,7 @@
     <row r="60">
       <c r="A60" s="1" t="inlineStr">
         <is>
-          <t>HR</t>
+          <t>Albumine</t>
         </is>
       </c>
       <c r="B60" t="n">
@@ -1038,17 +1038,17 @@
     <row r="61">
       <c r="A61" s="1" t="inlineStr">
         <is>
-          <t>Brief_CAR</t>
+          <t>RAD</t>
         </is>
       </c>
       <c r="B61" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="1" t="inlineStr">
         <is>
-          <t>Circulatory system</t>
+          <t>CAR</t>
         </is>
       </c>
       <c r="B62" t="n">
@@ -1058,7 +1058,7 @@
     <row r="63">
       <c r="A63" s="1" t="inlineStr">
         <is>
-          <t>CAR</t>
+          <t>AUD</t>
         </is>
       </c>
       <c r="B63" t="n">
@@ -1068,7 +1068,7 @@
     <row r="64">
       <c r="A64" s="1" t="inlineStr">
         <is>
-          <t>Iron-tablets</t>
+          <t>Dermatologic</t>
         </is>
       </c>
       <c r="B64" t="n">
@@ -1078,7 +1078,7 @@
     <row r="65">
       <c r="A65" s="1" t="inlineStr">
         <is>
-          <t>Mental disorders</t>
+          <t>TSH</t>
         </is>
       </c>
       <c r="B65" t="n">
@@ -1088,7 +1088,7 @@
     <row r="66">
       <c r="A66" s="1" t="inlineStr">
         <is>
-          <t>Brief_ONC</t>
+          <t>HR</t>
         </is>
       </c>
       <c r="B66" t="n">
@@ -1098,220 +1098,100 @@
     <row r="67">
       <c r="A67" s="1" t="inlineStr">
         <is>
-          <t>Injuries &amp; poisonings</t>
+          <t>Congenital anomalies</t>
         </is>
       </c>
       <c r="B67" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="1" t="inlineStr">
         <is>
-          <t>IMM</t>
+          <t>RTH</t>
         </is>
       </c>
       <c r="B68" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="1" t="inlineStr">
         <is>
-          <t>KEN</t>
+          <t>GGZ</t>
         </is>
       </c>
       <c r="B69" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="1" t="inlineStr">
         <is>
-          <t>Alk.Fosf.</t>
+          <t>Sense organs</t>
         </is>
       </c>
       <c r="B70" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="1" t="inlineStr">
         <is>
-          <t>Brief_CHI</t>
+          <t>HEM</t>
         </is>
       </c>
       <c r="B71" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="1" t="inlineStr">
         <is>
-          <t>NCH</t>
+          <t>FYS</t>
         </is>
       </c>
       <c r="B72" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="1" t="inlineStr">
         <is>
-          <t>Neurological</t>
+          <t>KNE</t>
         </is>
       </c>
       <c r="B73" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="1" t="inlineStr">
         <is>
-          <t>DER</t>
+          <t>NUC</t>
         </is>
       </c>
       <c r="B74" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="1" t="inlineStr">
         <is>
-          <t>Brief_RTH</t>
+          <t>Infectious diseases</t>
         </is>
       </c>
       <c r="B75" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="1" t="inlineStr">
         <is>
-          <t>PLA</t>
+          <t>Iron-tablets</t>
         </is>
       </c>
       <c r="B76" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="77">
-      <c r="A77" s="1" t="inlineStr">
-        <is>
-          <t>Dermatologic</t>
-        </is>
-      </c>
-      <c r="B77" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="78">
-      <c r="A78" s="1" t="inlineStr">
-        <is>
-          <t>Lipemische index</t>
-        </is>
-      </c>
-      <c r="B78" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="79">
-      <c r="A79" s="1" t="inlineStr">
-        <is>
-          <t>KIN</t>
-        </is>
-      </c>
-      <c r="B79" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="80">
-      <c r="A80" s="1" t="inlineStr">
-        <is>
-          <t>Brief_OOG</t>
-        </is>
-      </c>
-      <c r="B80" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="81">
-      <c r="A81" s="1" t="inlineStr">
-        <is>
-          <t>OOG</t>
-        </is>
-      </c>
-      <c r="B81" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="82">
-      <c r="A82" s="1" t="inlineStr">
-        <is>
-          <t>Brief_KNO</t>
-        </is>
-      </c>
-      <c r="B82" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="83">
-      <c r="A83" s="1" t="inlineStr">
-        <is>
-          <t>KCA</t>
-        </is>
-      </c>
-      <c r="B83" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="84">
-      <c r="A84" s="1" t="inlineStr">
-        <is>
-          <t>ORT</t>
-        </is>
-      </c>
-      <c r="B84" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="85">
-      <c r="A85" s="1" t="inlineStr">
-        <is>
-          <t>Brief_FYS</t>
-        </is>
-      </c>
-      <c r="B85" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="86">
-      <c r="A86" s="1" t="inlineStr">
-        <is>
-          <t>KCH</t>
-        </is>
-      </c>
-      <c r="B86" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="87">
-      <c r="A87" s="1" t="inlineStr">
-        <is>
-          <t>Brief_KEN</t>
-        </is>
-      </c>
-      <c r="B87" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="88">
-      <c r="A88" s="1" t="inlineStr">
-        <is>
-          <t>Brief_URO</t>
-        </is>
-      </c>
-      <c r="B88" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>